<commit_message>
groping the reperoting under dropdown list
</commit_message>
<xml_diff>
--- a/backend/src/reports/Report_AllWorkspaces_2025-10-16.xlsx
+++ b/backend/src/reports/Report_AllWorkspaces_2025-10-16.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Workspace</t>
   </si>
@@ -121,19 +121,7 @@
     <t>testing</t>
   </si>
   <si>
-    <t>hh vvv</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>MEDIUM</t>
-  </si>
-  <si>
-    <t>2025-10-30</t>
-  </si>
-  <si>
-    <t>rr</t>
+    <t>tt</t>
   </si>
 </sst>
 </file>
@@ -510,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F22"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="25" customWidth="1"/>
@@ -717,34 +705,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B22" t="s">
         <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>